<commit_message>
[WARNING] Dont Merge This Branch To Main Branch
</commit_message>
<xml_diff>
--- a/public/DataPengajar/pengajar.xlsx
+++ b/public/DataPengajar/pengajar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\PKL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D2CF41-802A-4923-AB1D-233CF71B84BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C896E678-B7BD-4920-8C57-947CE3438397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,44 +25,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
   <si>
     <t>Etika Profesi</t>
   </si>
   <si>
-    <t>Agung Raharja</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>Sistem Digital</t>
-  </si>
-  <si>
-    <t>Vida Mastrika</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>Struktur Data</t>
-  </si>
-  <si>
-    <t>Eka Karyawati</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>Kresna Dana</t>
-  </si>
-  <si>
-    <t>Algoritma Pemrograman</t>
-  </si>
-  <si>
     <t>kode_ajaran</t>
   </si>
   <si>
@@ -73,6 +52,111 @@
   </si>
   <si>
     <t>kelas_diampu</t>
+  </si>
+  <si>
+    <t>Cokorda Rai Adi Pramatha, S.T., M.M., Ph.D</t>
+  </si>
+  <si>
+    <t>Dr. Anak Agung Istri Ngurah Eka Karyawati, S.Si., M.Eng.</t>
+  </si>
+  <si>
+    <t>I Made Widiartha, S.Si., M. Kom</t>
+  </si>
+  <si>
+    <t>Dr. Dra. Luh Gede Astuti, M.Kom.</t>
+  </si>
+  <si>
+    <t>Algoritma &amp; Pemrograman</t>
+  </si>
+  <si>
+    <t>Dr. Made Agung Raharja, S.Si., M.Cs.</t>
+  </si>
+  <si>
+    <t>I Gusti Ngurah Anom Cahyadi Putra, ST., M.Cs</t>
+  </si>
+  <si>
+    <t>Dr. Ir. Ngurah Agus Sanjaya ER, S.Kom., M.Kom.</t>
+  </si>
+  <si>
+    <t>I Gede Santi Astawa, S.T., M.Cs.</t>
+  </si>
+  <si>
+    <t>Dr. Ir. I Ketut Gede Suhartana, S.Kom., M.Kom., IPM., ASEAN.Eng</t>
+  </si>
+  <si>
+    <t>Ida Ayu Gde Suwiprabayanti Putra, S.Kom., M.T.</t>
+  </si>
+  <si>
+    <t>I Putu Gede Hendra Suputra, S.Kom.,M.Kom.</t>
+  </si>
+  <si>
+    <t>I Made Widhi Wirawan, S.Si., M.Si., M.Cs.</t>
+  </si>
+  <si>
+    <t>Matematika Informatika</t>
+  </si>
+  <si>
+    <t>Kewarganegaraan</t>
+  </si>
+  <si>
+    <t>Bahasa Indonesia</t>
+  </si>
+  <si>
+    <t>Ilmu Sosial Dasar</t>
+  </si>
+  <si>
+    <t>Matematika Diskrit I</t>
+  </si>
+  <si>
+    <t>Interaksi Manusia dan Komputer</t>
+  </si>
+  <si>
+    <t>Basis Data</t>
+  </si>
+  <si>
+    <t>Desain dan Analisis Algoritma</t>
+  </si>
+  <si>
+    <t>Rekayasa Perangkat Lunak</t>
+  </si>
+  <si>
+    <t>Pemrograman Berorientasi Objek</t>
+  </si>
+  <si>
+    <t>Komunikasi Data dan Jaringan Komputer</t>
+  </si>
+  <si>
+    <t>Teori Bahasa dan Otomata</t>
+  </si>
+  <si>
+    <t>Komputer dan Masyarakat</t>
+  </si>
+  <si>
+    <t>Pemodelan dan Simulasi</t>
+  </si>
+  <si>
+    <t>Grafika Komputer</t>
+  </si>
+  <si>
+    <t>Sains Data</t>
+  </si>
+  <si>
+    <t>Basis Data Lanjut</t>
+  </si>
+  <si>
+    <t>Desain dan Pengujian Berpusat pada Pengguna</t>
+  </si>
+  <si>
+    <t>Teknologi Logika Fuzzy</t>
+  </si>
+  <si>
+    <t>Teknologi IOT</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -108,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -131,11 +215,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -145,6 +249,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,33 +551,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -463,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -474,13 +599,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -488,13 +613,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -502,16 +627,521 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
+      <c r="D20" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[UPDATE] Finallizing Genetic Algorithm for Scheduling
</commit_message>
<xml_diff>
--- a/public/DataPengajar/pengajar.xlsx
+++ b/public/DataPengajar/pengajar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C896E678-B7BD-4920-8C57-947CE3438397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62711D5-568D-470D-A578-FD52A54AE25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Etika Profesi</t>
   </si>
@@ -90,9 +90,6 @@
     <t>I Putu Gede Hendra Suputra, S.Kom.,M.Kom.</t>
   </si>
   <si>
-    <t>I Made Widhi Wirawan, S.Si., M.Si., M.Cs.</t>
-  </si>
-  <si>
     <t>Matematika Informatika</t>
   </si>
   <si>
@@ -145,12 +142,6 @@
   </si>
   <si>
     <t>Desain dan Pengujian Berpusat pada Pengguna</t>
-  </si>
-  <si>
-    <t>Teknologi Logika Fuzzy</t>
-  </si>
-  <si>
-    <t>Teknologi IOT</t>
   </si>
   <si>
     <t>B</t>
@@ -192,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -215,60 +206,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,58 +537,58 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -640,10 +596,10 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -654,24 +610,24 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -679,13 +635,13 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -693,13 +649,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -707,13 +663,13 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -721,27 +677,27 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -749,27 +705,27 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -777,13 +733,13 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -791,13 +747,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -805,13 +761,13 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -819,13 +775,13 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -833,27 +789,27 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -861,284 +817,124 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="8">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>2</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="8">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="8">
-        <v>36</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
-        <v>37</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>2</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
-        <v>38</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
-        <v>39</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
-        <v>40</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>